<commit_message>
bug with depicting multiple times one student fixed, excel file now making propertly
</commit_message>
<xml_diff>
--- a/public/hello world.xlsx
+++ b/public/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
   <si>
     <t>Шаблон</t>
   </si>
@@ -149,6 +149,12 @@
     <t>Дампилов Бимба Бимбаевич</t>
   </si>
   <si>
+    <t>Куулар Эдита Канкиевна</t>
+  </si>
+  <si>
+    <t>Ассистент</t>
+  </si>
+  <si>
     <t>Добрякова Снежана Дмитриевна</t>
   </si>
   <si>
@@ -195,6 +201,12 @@
   </si>
   <si>
     <t>АО "Байкалэнерго"</t>
+  </si>
+  <si>
+    <t>Аношко Алексей Федорович</t>
+  </si>
+  <si>
+    <t>Руководитель лаборатории сетевых систем и ИТ-инфраструктуры</t>
   </si>
   <si>
     <t>Пакулов Даниил Евгеньевич</t>
@@ -567,7 +579,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -842,6 +854,12 @@
       <c r="D24" t="s">
         <v>36</v>
       </c>
+      <c r="H24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25">
@@ -851,7 +869,7 @@
         <v>4566</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
         <v>36</v>
@@ -865,7 +883,7 @@
         <v>4567</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
         <v>36</v>
@@ -879,7 +897,7 @@
         <v>4568</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
         <v>36</v>
@@ -893,7 +911,7 @@
         <v>4569</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
         <v>36</v>
@@ -907,7 +925,7 @@
         <v>4570</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
         <v>36</v>
@@ -921,7 +939,7 @@
         <v>4571</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
         <v>36</v>
@@ -935,7 +953,7 @@
         <v>4572</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
         <v>36</v>
@@ -949,7 +967,7 @@
         <v>4573</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
         <v>36</v>
@@ -963,7 +981,7 @@
         <v>4574</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
         <v>36</v>
@@ -977,7 +995,7 @@
         <v>4575</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -991,7 +1009,7 @@
         <v>4576</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
         <v>36</v>
@@ -1005,7 +1023,7 @@
         <v>4577</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D36" t="s">
         <v>36</v>
@@ -1019,7 +1037,7 @@
         <v>4578</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
         <v>36</v>
@@ -1033,7 +1051,7 @@
         <v>4579</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
         <v>36</v>
@@ -1047,13 +1065,19 @@
         <v>4580</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
         <v>36</v>
       </c>
       <c r="E39" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="H39" t="s">
+        <v>62</v>
+      </c>
+      <c r="I39" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1064,7 +1088,7 @@
         <v>4581</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D40" t="s">
         <v>36</v>
@@ -1078,7 +1102,7 @@
         <v>4582</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D41" t="s">
         <v>36</v>
@@ -1092,7 +1116,7 @@
         <v>4583</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
         <v>36</v>
@@ -1106,7 +1130,7 @@
         <v>4584</v>
       </c>
       <c r="C43" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D43" t="s">
         <v>36</v>
@@ -1120,7 +1144,7 @@
         <v>4585</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D44" t="s">
         <v>36</v>
@@ -1134,7 +1158,7 @@
         <v>4586</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D45" t="s">
         <v>36</v>
@@ -1148,7 +1172,7 @@
         <v>4587</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D46" t="s">
         <v>36</v>
@@ -1162,7 +1186,7 @@
         <v>4588</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D47" t="s">
         <v>36</v>
@@ -1176,7 +1200,7 @@
         <v>4589</v>
       </c>
       <c r="C48" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D48" t="s">
         <v>36</v>
@@ -1190,7 +1214,7 @@
         <v>4590</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D49" t="s">
         <v>36</v>
@@ -1204,10 +1228,18 @@
         <v>4591</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D50" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="H90">
+        <v>121</v>
+      </c>
+      <c r="I90">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>